<commit_message>
examples - RDF, HTML index, embed anywhere
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/ucr.xlsx
+++ b/documentation-generator/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -136,7 +136,13 @@
     <t>The concepts should be bundled together and provided as a vocabulary or thesauri with distinct parts or sections (or sub-vocabularies) that relate to specific contextual details. For example, providing purposes as a separate taxonomy enables use of only purposes elsewhere.</t>
   </si>
   <si>
-    <t>Source path</t>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>SourceFormat</t>
+  </si>
+  <si>
+    <t>SourceType</t>
   </si>
   <si>
     <t>Concepts</t>
@@ -145,7 +151,7 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Embed?</t>
+    <t>Status</t>
   </si>
   <si>
     <t>E0001</t>
@@ -160,10 +166,16 @@
     <t>E0001.ttl</t>
   </si>
   <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>ttl</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>dpv:Purpose</t>
+  </si>
+  <si>
+    <t>accepted</t>
   </si>
   <si>
     <t>Harsh</t>
@@ -181,9 +193,6 @@
     <t>E0002.ttl</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>E0003</t>
   </si>
   <si>
@@ -196,9 +205,6 @@
     <t>E0003.ttl</t>
   </si>
   <si>
-    <t>dpvs:Purpose</t>
-  </si>
-  <si>
     <t>E0004</t>
   </si>
   <si>
@@ -208,9 +214,6 @@
     <t>E0004.ttl</t>
   </si>
   <si>
-    <t>dpvo:Purpose</t>
-  </si>
-  <si>
     <t>E0005</t>
   </si>
   <si>
@@ -223,7 +226,7 @@
     <t>E0005.ttl</t>
   </si>
   <si>
-    <t>dpv:Concept,dpv:Processing</t>
+    <t>dpv:Processing</t>
   </si>
   <si>
     <t>E0006</t>
@@ -238,9 +241,6 @@
     <t>E0006.ttl</t>
   </si>
   <si>
-    <t>dpv:Concept,dpv:Purpose</t>
-  </si>
-  <si>
     <t>E0007</t>
   </si>
   <si>
@@ -337,7 +337,7 @@
     <t>E0013.ttl</t>
   </si>
   <si>
-    <t>dpv:ProcessingAutomation,dpv:HumanInput</t>
+    <t>dpv:Automation</t>
   </si>
   <si>
     <t>E0014</t>
@@ -382,7 +382,7 @@
     <t>E0016.ttl</t>
   </si>
   <si>
-    <t>dpv:TechnicalMeasure,dpv:Encryption,dpv:AccessControlMethod</t>
+    <t>dpv:Encryption,dpv:AccessControlMethod</t>
   </si>
   <si>
     <t>E0017</t>
@@ -397,7 +397,7 @@
     <t>E0017.ttl</t>
   </si>
   <si>
-    <t>dpv:OrganisationalMeasure,dpv:StaffTraining,dpv:Policy</t>
+    <t>dpv:StaffTraining,dpv:Policy</t>
   </si>
   <si>
     <t>E0018</t>
@@ -442,7 +442,7 @@
     <t>E0020.ttl</t>
   </si>
   <si>
-    <t>dpv:Controller,dpv:Processor,dpv:ControllerProcessorAgreement,dpv:PersonalDataHandling,dpv:Transfer,dpv:DataSource</t>
+    <t>dpv:DataController,dpv:ControllerProcessor,dpv:ControllerProcessorAgreement,dpv:PersonalDataHandling,dpv:Transfer,dpv:DataSource</t>
   </si>
   <si>
     <t>E0021</t>
@@ -457,7 +457,7 @@
     <t>E0021.ttl</t>
   </si>
   <si>
-    <t>dpv:ControllerProcessorAgreement,dpv:DataTransferSafeguard,dpv-gdpr:SCCsByCommission</t>
+    <t>dpv:ControllerProcessorAgreement,dpv:DataTransferSafeguard,eu-gdpr:SCCsByCommission</t>
   </si>
   <si>
     <t>E0022</t>
@@ -574,7 +574,7 @@
     <t>E0029.ttl</t>
   </si>
   <si>
-    <t>dpv:Riskl,dpv:Consequence,dpv:Impact,dpv:Harm,dpv:RiskMitigationMeasure</t>
+    <t>dpv:Risk,dpv:Consequence,dpv:Impact,dpv:Harm,dpv:RiskMitigationMeasure</t>
   </si>
   <si>
     <t>EXAMPLE</t>
@@ -1173,7 +1173,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1182,7 +1182,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>41</v>
@@ -1194,13 +1194,17 @@
         <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1216,37 +1220,41 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="6">
+        <v>52</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="6">
         <v>44846.0</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -1262,37 +1270,41 @@
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="6">
         <v>44846.0</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -1308,121 +1320,138 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>48</v>
+      <c r="E6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>48</v>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -1438,20 +1467,24 @@
       <c r="D8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>50</v>
+      <c r="H8" s="9"/>
+      <c r="I8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9">
@@ -1467,20 +1500,24 @@
       <c r="D9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>50</v>
+      <c r="H9" s="9"/>
+      <c r="I9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -1496,20 +1533,24 @@
       <c r="D10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>48</v>
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11">
@@ -1525,20 +1566,24 @@
       <c r="D11" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>50</v>
+      <c r="H11" s="9"/>
+      <c r="I11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12">
@@ -1554,20 +1599,24 @@
       <c r="D12" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>50</v>
+      <c r="H12" s="9"/>
+      <c r="I12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -1583,20 +1632,24 @@
       <c r="D13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>50</v>
+      <c r="H13" s="9"/>
+      <c r="I13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -1612,20 +1665,24 @@
       <c r="D14" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>50</v>
+      <c r="H14" s="9"/>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15">
@@ -1641,20 +1698,24 @@
       <c r="D15" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>50</v>
+      <c r="H15" s="9"/>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16">
@@ -1670,20 +1731,24 @@
       <c r="D16" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>50</v>
+      <c r="H16" s="9"/>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17">
@@ -1699,20 +1764,24 @@
       <c r="D17" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>50</v>
+      <c r="H17" s="9"/>
+      <c r="I17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18">
@@ -1728,20 +1797,24 @@
       <c r="D18" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>50</v>
+      <c r="H18" s="9"/>
+      <c r="I18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19">
@@ -1757,20 +1830,24 @@
       <c r="D19" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>50</v>
+      <c r="H19" s="9"/>
+      <c r="I19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20">
@@ -1786,20 +1863,24 @@
       <c r="D20" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>50</v>
+      <c r="H20" s="9"/>
+      <c r="I20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21">
@@ -1815,20 +1896,24 @@
       <c r="D21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>50</v>
+      <c r="H21" s="9"/>
+      <c r="I21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22">
@@ -1844,20 +1929,24 @@
       <c r="D22" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>50</v>
+      <c r="H22" s="9"/>
+      <c r="I22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23">
@@ -1873,20 +1962,24 @@
       <c r="D23" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>50</v>
+      <c r="H23" s="9"/>
+      <c r="I23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24">
@@ -1902,20 +1995,24 @@
       <c r="D24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>50</v>
+      <c r="H24" s="9"/>
+      <c r="I24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25">
@@ -1931,20 +2028,24 @@
       <c r="D25" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>50</v>
+      <c r="H25" s="9"/>
+      <c r="I25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26">
@@ -1960,20 +2061,24 @@
       <c r="D26" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>50</v>
+      <c r="H26" s="9"/>
+      <c r="I26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27">
@@ -1989,20 +2094,24 @@
       <c r="D27" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>50</v>
+      <c r="H27" s="9"/>
+      <c r="I27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28">
@@ -2018,20 +2127,24 @@
       <c r="D28" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>50</v>
+      <c r="H28" s="9"/>
+      <c r="I28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29">
@@ -2047,20 +2160,24 @@
       <c r="D29" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>50</v>
+      <c r="H29" s="9"/>
+      <c r="I29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="10">
+        <v>44847.0</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30">
@@ -2076,20 +2193,24 @@
       <c r="D30" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="8">
-        <v>44847.0</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>50</v>
+      <c r="H30" s="9"/>
+      <c r="I30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="8">
+        <v>44847.0</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>